<commit_message>
Corrected one excel file!!
</commit_message>
<xml_diff>
--- a/First iteration/data/ES39.xlsx
+++ b/First iteration/data/ES39.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Filename</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>Datei enthält 12 Gangepisoden, Kompassspur irgendwie komisch</t>
-  </si>
-  <si>
-    <t>Datei enthält 11 Gangepisoden</t>
   </si>
 </sst>
 </file>
@@ -965,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:I26"/>
+      <selection activeCell="A17" sqref="A17:AG17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,11 +1139,6 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K17" t="s">
-        <v>39</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>

</xml_diff>